<commit_message>
Uploading the files for the thesis
</commit_message>
<xml_diff>
--- a/COUNTRY_GENERAL.xlsx
+++ b/COUNTRY_GENERAL.xlsx
@@ -515,7 +515,7 @@
         <v>0.309</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4990829027363295</v>
+        <v>0.4990599252230002</v>
       </c>
     </row>
     <row r="3">
@@ -553,7 +553,7 @@
         <v>0.298</v>
       </c>
       <c r="J3" t="n">
-        <v>0.282105179494283</v>
+        <v>0.2820613066717299</v>
       </c>
     </row>
     <row r="4">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1476169265391374</v>
+        <v>0.1476426129932199</v>
       </c>
     </row>
     <row r="5">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4198058255572675</v>
+        <v>0.4217541131094461</v>
       </c>
     </row>
     <row r="6">
@@ -667,7 +667,7 @@
         <v>0.176</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2164628273680946</v>
+        <v>0.2164461266178898</v>
       </c>
     </row>
     <row r="7">
@@ -705,7 +705,7 @@
         <v>0.288</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4301436015734804</v>
+        <v>0.4301034542156687</v>
       </c>
     </row>
     <row r="8">
@@ -743,7 +743,7 @@
         <v>0.101</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2406633112218168</v>
+        <v>0.2406804510048449</v>
       </c>
     </row>
     <row r="9">
@@ -778,10 +778,10 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01793394695301773</v>
+        <v>0.01848812080391261</v>
       </c>
     </row>
     <row r="10">
@@ -854,10 +854,10 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4654986248737465</v>
+        <v>0.4644775990715255</v>
       </c>
     </row>
     <row r="12">
@@ -895,7 +895,7 @@
         <v>0.101</v>
       </c>
       <c r="J12" t="n">
-        <v>0.02244017078330028</v>
+        <v>0.02239719540181203</v>
       </c>
     </row>
     <row r="13">
@@ -933,7 +933,7 @@
         <v>0.298</v>
       </c>
       <c r="J13" t="n">
-        <v>0.303964919276116</v>
+        <v>0.3039556092887007</v>
       </c>
     </row>
     <row r="14">
@@ -1009,7 +1009,7 @@
         <v>0.176</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1039297924153769</v>
+        <v>0.1039398781687476</v>
       </c>
     </row>
     <row r="16">
@@ -1047,7 +1047,7 @@
         <v>0.151</v>
       </c>
       <c r="J16" t="n">
-        <v>0.04079065426433658</v>
+        <v>0.04072492600419058</v>
       </c>
     </row>
     <row r="17">
@@ -1085,7 +1085,7 @@
         <v>0.309</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1735651231463367</v>
+        <v>0.1735707412293278</v>
       </c>
     </row>
     <row r="18">
@@ -1120,10 +1120,10 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0196459619291064</v>
+        <v>0.02252056539934649</v>
       </c>
     </row>
     <row r="19">
@@ -1161,7 +1161,7 @@
         <v>0.134</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2805705380177575</v>
+        <v>0.280608076675635</v>
       </c>
     </row>
     <row r="20">
@@ -1196,10 +1196,10 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J20" t="n">
-        <v>0.330895192955994</v>
+        <v>0.3302262478753878</v>
       </c>
     </row>
     <row r="21">
@@ -1237,7 +1237,7 @@
         <v>0.298</v>
       </c>
       <c r="J21" t="n">
-        <v>0.425760637360719</v>
+        <v>0.4257637267155437</v>
       </c>
     </row>
     <row r="22">
@@ -1275,7 +1275,7 @@
         <v>0.298</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5080856207380079</v>
+        <v>0.5076638709103816</v>
       </c>
     </row>
     <row r="23">
@@ -1313,7 +1313,7 @@
         <v>0.101</v>
       </c>
       <c r="J23" t="n">
-        <v>0.04152533384715174</v>
+        <v>0.04157775284895771</v>
       </c>
     </row>
     <row r="24">
@@ -1351,7 +1351,7 @@
         <v>0.309</v>
       </c>
       <c r="J24" t="n">
-        <v>0.4953130667358765</v>
+        <v>0.4953227011316043</v>
       </c>
     </row>
     <row r="25">
@@ -1389,7 +1389,7 @@
         <v>0.101</v>
       </c>
       <c r="J25" t="n">
-        <v>0.07949745427559909</v>
+        <v>0.07953569617793384</v>
       </c>
     </row>
     <row r="26">
@@ -1503,7 +1503,7 @@
         <v>0.309</v>
       </c>
       <c r="J28" t="n">
-        <v>0.4196339956736317</v>
+        <v>0.4196108196424674</v>
       </c>
     </row>
     <row r="29">
@@ -1541,7 +1541,7 @@
         <v>-0.024</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.08318194510247962</v>
+        <v>-0.08326597807506439</v>
       </c>
     </row>
     <row r="30">
@@ -1576,10 +1576,10 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J30" t="n">
-        <v>0.3234064212287931</v>
+        <v>0.323409311750511</v>
       </c>
     </row>
     <row r="31">
@@ -1617,7 +1617,7 @@
         <v>0.176</v>
       </c>
       <c r="J31" t="n">
-        <v>0.2367062806121736</v>
+        <v>0.2367224458284039</v>
       </c>
     </row>
     <row r="32">
@@ -1652,10 +1652,10 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J32" t="n">
-        <v>0.4078143365568883</v>
+        <v>0.4096935125152908</v>
       </c>
     </row>
     <row r="33">
@@ -1690,10 +1690,10 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.01267817679064375</v>
+        <v>-0.01267755319656486</v>
       </c>
     </row>
     <row r="34">
@@ -1731,7 +1731,7 @@
         <v>0.316</v>
       </c>
       <c r="J34" t="n">
-        <v>0.292046703443701</v>
+        <v>0.2919773934154427</v>
       </c>
     </row>
     <row r="35">
@@ -1766,10 +1766,10 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J35" t="n">
-        <v>0.01785951271588301</v>
+        <v>0.02145274694547699</v>
       </c>
     </row>
     <row r="36">
@@ -1807,7 +1807,7 @@
         <v>0.303</v>
       </c>
       <c r="J36" t="n">
-        <v>0.05706462838410328</v>
+        <v>0.05703559743261691</v>
       </c>
     </row>
     <row r="37">
@@ -1845,7 +1845,7 @@
         <v>0.298</v>
       </c>
       <c r="J37" t="n">
-        <v>0.4786010770273145</v>
+        <v>0.47825177785425</v>
       </c>
     </row>
     <row r="38">
@@ -1883,7 +1883,7 @@
         <v>0.16</v>
       </c>
       <c r="J38" t="n">
-        <v>0.1250001482754089</v>
+        <v>0.1250177299905346</v>
       </c>
     </row>
     <row r="39">
@@ -1921,7 +1921,7 @@
         <v>0.309</v>
       </c>
       <c r="J39" t="n">
-        <v>0.4061311807675869</v>
+        <v>0.4061397196405911</v>
       </c>
     </row>
     <row r="40">
@@ -1959,7 +1959,7 @@
         <v>0.298</v>
       </c>
       <c r="J40" t="n">
-        <v>0.1096152235231872</v>
+        <v>0.1095806013756176</v>
       </c>
     </row>
     <row r="41">
@@ -1997,7 +1997,7 @@
         <v>0.101</v>
       </c>
       <c r="J41" t="n">
-        <v>0.1186796983395722</v>
+        <v>0.1186553737098471</v>
       </c>
     </row>
     <row r="42">
@@ -2073,7 +2073,7 @@
         <v>0.275</v>
       </c>
       <c r="J43" t="n">
-        <v>0.3026562157140181</v>
+        <v>0.3023694523425924</v>
       </c>
     </row>
     <row r="44">
@@ -2108,10 +2108,10 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J44" t="n">
-        <v>0.5007629086625632</v>
+        <v>0.5007610596731203</v>
       </c>
     </row>
     <row r="45">
@@ -2146,10 +2146,10 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J45" t="n">
-        <v>0.5099390499006524</v>
+        <v>0.5090248477388138</v>
       </c>
     </row>
     <row r="46">
@@ -2184,10 +2184,10 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J46" t="n">
-        <v>-0.04413485822558975</v>
+        <v>-0.04118040467645769</v>
       </c>
     </row>
     <row r="47">
@@ -2225,7 +2225,7 @@
         <v>0.298</v>
       </c>
       <c r="J47" t="n">
-        <v>0.4359435621393236</v>
+        <v>0.43592317478254</v>
       </c>
     </row>
     <row r="48">
@@ -2260,10 +2260,10 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J48" t="n">
-        <v>0.3785202206928028</v>
+        <v>0.3811316671204216</v>
       </c>
     </row>
     <row r="49">
@@ -2301,7 +2301,7 @@
         <v>0.316</v>
       </c>
       <c r="J49" t="n">
-        <v>0.2212666007433389</v>
+        <v>0.2212940524895317</v>
       </c>
     </row>
     <row r="50">
@@ -2339,7 +2339,7 @@
         <v>0.309</v>
       </c>
       <c r="J50" t="n">
-        <v>0.4266779206172277</v>
+        <v>0.426687566770301</v>
       </c>
     </row>
     <row r="51">
@@ -2374,10 +2374,10 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J51" t="n">
-        <v>0.5114508114228847</v>
+        <v>0.5105892490881661</v>
       </c>
     </row>
     <row r="52">
@@ -2491,7 +2491,7 @@
         <v>0.176</v>
       </c>
       <c r="J54" t="n">
-        <v>0.0588252747538841</v>
+        <v>0.05879748186741546</v>
       </c>
     </row>
     <row r="55">
@@ -2529,7 +2529,7 @@
         <v>0.277</v>
       </c>
       <c r="J55" t="n">
-        <v>0.1613796289877275</v>
+        <v>0.1613451644303059</v>
       </c>
     </row>
     <row r="56">
@@ -2567,7 +2567,7 @@
         <v>0.298</v>
       </c>
       <c r="J56" t="n">
-        <v>0.2687922028480548</v>
+        <v>0.2687822320479302</v>
       </c>
     </row>
     <row r="57">
@@ -2605,7 +2605,7 @@
         <v>0.073</v>
       </c>
       <c r="J57" t="n">
-        <v>0.110826291279706</v>
+        <v>0.1107397378177327</v>
       </c>
     </row>
     <row r="58">
@@ -2643,7 +2643,7 @@
         <v>0.298</v>
       </c>
       <c r="J58" t="n">
-        <v>0.03617218243458033</v>
+        <v>0.03613275982217706</v>
       </c>
     </row>
     <row r="59">
@@ -2681,7 +2681,7 @@
         <v>0.277</v>
       </c>
       <c r="J59" t="n">
-        <v>-0.006142152164076481</v>
+        <v>-0.006257490557445134</v>
       </c>
     </row>
     <row r="60">
@@ -2716,10 +2716,10 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J60" t="n">
-        <v>0.5285849446895156</v>
+        <v>0.5285957538646354</v>
       </c>
     </row>
     <row r="61">
@@ -2757,7 +2757,7 @@
         <v>0.288</v>
       </c>
       <c r="J61" t="n">
-        <v>0.3814701128752561</v>
+        <v>0.3814031631509821</v>
       </c>
     </row>
     <row r="62">
@@ -2792,10 +2792,10 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J62" t="n">
-        <v>0.2299704868225448</v>
+        <v>0.2323989823870055</v>
       </c>
     </row>
     <row r="63">
@@ -2833,7 +2833,7 @@
         <v>0.288</v>
       </c>
       <c r="J63" t="n">
-        <v>0.1406800964772588</v>
+        <v>0.1406428816611889</v>
       </c>
     </row>
     <row r="64">
@@ -2871,7 +2871,7 @@
         <v>0.298</v>
       </c>
       <c r="J64" t="n">
-        <v>0.1356636028286416</v>
+        <v>0.1347736765295389</v>
       </c>
     </row>
     <row r="65">
@@ -2909,7 +2909,7 @@
         <v>0.303</v>
       </c>
       <c r="J65" t="n">
-        <v>0.5164422504724425</v>
+        <v>0.5164440580621827</v>
       </c>
     </row>
     <row r="66">
@@ -2947,7 +2947,7 @@
         <v>0.134</v>
       </c>
       <c r="J66" t="n">
-        <v>0.06326064536347674</v>
+        <v>0.06323565110363584</v>
       </c>
     </row>
     <row r="67">
@@ -2985,7 +2985,7 @@
         <v>0.432</v>
       </c>
       <c r="J67" t="n">
-        <v>0.2824831915915237</v>
+        <v>0.2824872624458036</v>
       </c>
     </row>
     <row r="68">
@@ -3023,7 +3023,7 @@
         <v>0.288</v>
       </c>
       <c r="J68" t="n">
-        <v>0.2299605359619578</v>
+        <v>0.2299417725987154</v>
       </c>
     </row>
     <row r="69">
@@ -3058,10 +3058,10 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J69" t="n">
-        <v>0.3577708800419133</v>
+        <v>0.356979435303258</v>
       </c>
     </row>
     <row r="70">
@@ -3096,10 +3096,10 @@
         </is>
       </c>
       <c r="I70" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J70" t="n">
-        <v>0.3843859995426117</v>
+        <v>0.3843521135118149</v>
       </c>
     </row>
     <row r="71">
@@ -3137,7 +3137,7 @@
         <v>0.073</v>
       </c>
       <c r="J71" t="n">
-        <v>0.1396245135737843</v>
+        <v>0.1395752388762919</v>
       </c>
     </row>
     <row r="72">
@@ -3175,7 +3175,7 @@
         <v>0.148</v>
       </c>
       <c r="J72" t="n">
-        <v>0.4153656750416387</v>
+        <v>0.4153821671577619</v>
       </c>
     </row>
     <row r="73">
@@ -3213,7 +3213,7 @@
         <v>0.148</v>
       </c>
       <c r="J73" t="n">
-        <v>0.03347822158799613</v>
+        <v>0.03354714960432352</v>
       </c>
     </row>
     <row r="74">
@@ -3251,7 +3251,7 @@
         <v>0.288</v>
       </c>
       <c r="J74" t="n">
-        <v>0.1949042322439054</v>
+        <v>0.1948209916912795</v>
       </c>
     </row>
     <row r="75">
@@ -3289,7 +3289,7 @@
         <v>0.277</v>
       </c>
       <c r="J75" t="n">
-        <v>0.4764140209644951</v>
+        <v>0.4764222009842473</v>
       </c>
     </row>
     <row r="76">
@@ -3327,7 +3327,7 @@
         <v>0.398</v>
       </c>
       <c r="J76" t="n">
-        <v>0.4364574077478077</v>
+        <v>0.4364512086665305</v>
       </c>
     </row>
     <row r="77">
@@ -3365,7 +3365,7 @@
         <v>0.151</v>
       </c>
       <c r="J77" t="n">
-        <v>0.1859966507595695</v>
+        <v>0.1860802591295749</v>
       </c>
     </row>
     <row r="78">
@@ -3403,7 +3403,7 @@
         <v>0.188</v>
       </c>
       <c r="J78" t="n">
-        <v>0.2767056039786749</v>
+        <v>0.276697504831985</v>
       </c>
     </row>
     <row r="79">
@@ -3438,10 +3438,10 @@
         </is>
       </c>
       <c r="I79" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J79" t="n">
-        <v>0.02443939023919282</v>
+        <v>0.02629351453809277</v>
       </c>
     </row>
     <row r="80">
@@ -3479,7 +3479,7 @@
         <v>0.176</v>
       </c>
       <c r="J80" t="n">
-        <v>0.2832752608334032</v>
+        <v>0.283219598574018</v>
       </c>
     </row>
     <row r="81">
@@ -3514,10 +3514,10 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J81" t="n">
-        <v>0.2355135870124031</v>
+        <v>0.2355191101275094</v>
       </c>
     </row>
     <row r="82">
@@ -3555,7 +3555,7 @@
         <v>0.148</v>
       </c>
       <c r="J82" t="n">
-        <v>0.276310618065418</v>
+        <v>0.2763374891632372</v>
       </c>
     </row>
     <row r="83">
@@ -3593,7 +3593,7 @@
         <v>0.203</v>
       </c>
       <c r="J83" t="n">
-        <v>0.1929829580208898</v>
+        <v>0.1929761472770076</v>
       </c>
     </row>
     <row r="84">
@@ -3631,7 +3631,7 @@
         <v>-0.024</v>
       </c>
       <c r="J84" t="n">
-        <v>0.1509798798864222</v>
+        <v>0.1509760503011331</v>
       </c>
     </row>
     <row r="85">
@@ -3707,7 +3707,7 @@
         <v>0.188</v>
       </c>
       <c r="J86" t="n">
-        <v>0.119328029929763</v>
+        <v>0.1193305813195456</v>
       </c>
     </row>
     <row r="87">
@@ -3745,7 +3745,7 @@
         <v>0.176</v>
       </c>
       <c r="J87" t="n">
-        <v>0.3720926326663825</v>
+        <v>0.3721231892409765</v>
       </c>
     </row>
     <row r="88">
@@ -3783,7 +3783,7 @@
         <v>0.148</v>
       </c>
       <c r="J88" t="n">
-        <v>0.1794369411694574</v>
+        <v>0.179442565718145</v>
       </c>
     </row>
     <row r="89">
@@ -3821,7 +3821,7 @@
         <v>0.303</v>
       </c>
       <c r="J89" t="n">
-        <v>0.5089678673629164</v>
+        <v>0.5089721942993435</v>
       </c>
     </row>
     <row r="90">
@@ -3859,7 +3859,7 @@
         <v>0.275</v>
       </c>
       <c r="J90" t="n">
-        <v>0.309268020934659</v>
+        <v>0.309211511426598</v>
       </c>
     </row>
     <row r="91">
@@ -3897,7 +3897,7 @@
         <v>0.623</v>
       </c>
       <c r="J91" t="n">
-        <v>0.3744171387945047</v>
+        <v>0.3744054346875522</v>
       </c>
     </row>
     <row r="92">
@@ -3935,7 +3935,7 @@
         <v>0.309</v>
       </c>
       <c r="J92" t="n">
-        <v>0.1781486177785682</v>
+        <v>0.1781088505415076</v>
       </c>
     </row>
     <row r="93">
@@ -3973,7 +3973,7 @@
         <v>0.432</v>
       </c>
       <c r="J93" t="n">
-        <v>0.3281781487563332</v>
+        <v>0.3282543335006137</v>
       </c>
     </row>
     <row r="94">
@@ -4011,7 +4011,7 @@
         <v>-0.024</v>
       </c>
       <c r="J94" t="n">
-        <v>-0.05423727588115813</v>
+        <v>-0.05428021051746645</v>
       </c>
     </row>
     <row r="95">
@@ -4046,10 +4046,10 @@
         </is>
       </c>
       <c r="I95" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J95" t="n">
-        <v>0.1942308843683669</v>
+        <v>0.194227339338198</v>
       </c>
     </row>
     <row r="96">
@@ -4087,7 +4087,7 @@
         <v>0.288</v>
       </c>
       <c r="J96" t="n">
-        <v>0.3483825422341318</v>
+        <v>0.3483696194323307</v>
       </c>
     </row>
     <row r="97">
@@ -4125,7 +4125,7 @@
         <v>0.177</v>
       </c>
       <c r="J97" t="n">
-        <v>0.238053737940328</v>
+        <v>0.238055921485226</v>
       </c>
     </row>
     <row r="98">
@@ -4160,10 +4160,10 @@
         </is>
       </c>
       <c r="I98" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J98" t="n">
-        <v>0.2183978179054354</v>
+        <v>0.2251446953529576</v>
       </c>
     </row>
     <row r="99">
@@ -4201,7 +4201,7 @@
         <v>0.203</v>
       </c>
       <c r="J99" t="n">
-        <v>0.3266147312369694</v>
+        <v>0.3266045458776838</v>
       </c>
     </row>
     <row r="100">
@@ -4239,7 +4239,7 @@
         <v>0.148</v>
       </c>
       <c r="J100" t="n">
-        <v>-0.02097654850544095</v>
+        <v>-0.02099104418538274</v>
       </c>
     </row>
     <row r="101">
@@ -4274,10 +4274,10 @@
         </is>
       </c>
       <c r="I101" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J101" t="n">
-        <v>0.2546156984037769</v>
+        <v>0.2546162250546257</v>
       </c>
     </row>
     <row r="102">
@@ -4315,7 +4315,7 @@
         <v>0.134</v>
       </c>
       <c r="J102" t="n">
-        <v>-0.01337721291908661</v>
+        <v>-0.01337510737328314</v>
       </c>
     </row>
     <row r="103">
@@ -4353,7 +4353,7 @@
         <v>0.398</v>
       </c>
       <c r="J103" t="n">
-        <v>0.358621573619693</v>
+        <v>0.3585913765386816</v>
       </c>
     </row>
     <row r="104">
@@ -4391,7 +4391,7 @@
         <v>0.073</v>
       </c>
       <c r="J104" t="n">
-        <v>0.1099769886832349</v>
+        <v>0.1099442550052648</v>
       </c>
     </row>
     <row r="105">
@@ -4429,7 +4429,7 @@
         <v>0.277</v>
       </c>
       <c r="J105" t="n">
-        <v>0.3803815698166342</v>
+        <v>0.3803534100722884</v>
       </c>
     </row>
     <row r="106">
@@ -4467,7 +4467,7 @@
         <v>0.148</v>
       </c>
       <c r="J106" t="n">
-        <v>0.1492836538460391</v>
+        <v>0.1492587680013551</v>
       </c>
     </row>
     <row r="107">
@@ -4505,7 +4505,7 @@
         <v>0.176</v>
       </c>
       <c r="J107" t="n">
-        <v>-0.04048139109350558</v>
+        <v>-0.0404970629304991</v>
       </c>
     </row>
     <row r="108">
@@ -4543,7 +4543,7 @@
         <v>0.309</v>
       </c>
       <c r="J108" t="n">
-        <v>0.1510470563870555</v>
+        <v>0.1510777045539319</v>
       </c>
     </row>
     <row r="109">
@@ -4581,7 +4581,7 @@
         <v>0.177</v>
       </c>
       <c r="J109" t="n">
-        <v>0.183089737479151</v>
+        <v>0.1831403125384959</v>
       </c>
     </row>
     <row r="110">
@@ -4616,10 +4616,10 @@
         </is>
       </c>
       <c r="I110" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J110" t="n">
-        <v>0.3115352747324975</v>
+        <v>0.3105145591376559</v>
       </c>
     </row>
     <row r="111">
@@ -4657,7 +4657,7 @@
         <v>0.316</v>
       </c>
       <c r="J111" t="n">
-        <v>0.4186625996838523</v>
+        <v>0.4186652770476801</v>
       </c>
     </row>
     <row r="112">
@@ -4695,7 +4695,7 @@
         <v>0.316</v>
       </c>
       <c r="J112" t="n">
-        <v>0.343837943430027</v>
+        <v>0.3438383820440475</v>
       </c>
     </row>
     <row r="113">
@@ -4733,7 +4733,7 @@
         <v>0.505</v>
       </c>
       <c r="J113" t="n">
-        <v>0.2196085281555691</v>
+        <v>0.2196202959409533</v>
       </c>
     </row>
     <row r="114">
@@ -4771,7 +4771,7 @@
         <v>0.546</v>
       </c>
       <c r="J114" t="n">
-        <v>0.5581508778329772</v>
+        <v>0.5581626345282948</v>
       </c>
     </row>
     <row r="115">
@@ -4809,7 +4809,7 @@
         <v>0.316</v>
       </c>
       <c r="J115" t="n">
-        <v>0.1371934376283371</v>
+        <v>0.1371939455386838</v>
       </c>
     </row>
     <row r="116">
@@ -4847,7 +4847,7 @@
         <v>0.275</v>
       </c>
       <c r="J116" t="n">
-        <v>0.146810404295992</v>
+        <v>0.1455780738870461</v>
       </c>
     </row>
     <row r="117">
@@ -4885,7 +4885,7 @@
         <v>0.316</v>
       </c>
       <c r="J117" t="n">
-        <v>0.4859784758924938</v>
+        <v>0.4859721745941007</v>
       </c>
     </row>
     <row r="118">
@@ -4923,7 +4923,7 @@
         <v>0.177</v>
       </c>
       <c r="J118" t="n">
-        <v>0.1372812934415644</v>
+        <v>0.1372765630244224</v>
       </c>
     </row>
     <row r="119">
@@ -4958,10 +4958,10 @@
         </is>
       </c>
       <c r="I119" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J119" t="n">
-        <v>0.3207129595697441</v>
+        <v>0.3206939196704131</v>
       </c>
     </row>
     <row r="120">
@@ -4999,7 +4999,7 @@
         <v>0.252</v>
       </c>
       <c r="J120" t="n">
-        <v>0.2600869949377427</v>
+        <v>0.2601151314709095</v>
       </c>
     </row>
     <row r="121">
@@ -5034,10 +5034,10 @@
         </is>
       </c>
       <c r="I121" t="n">
-        <v>0.298</v>
+        <v>0.297</v>
       </c>
       <c r="J121" t="n">
-        <v>0.03516634734217502</v>
+        <v>0.03350859723147322</v>
       </c>
     </row>
     <row r="122">
@@ -5075,7 +5075,7 @@
         <v>0.275</v>
       </c>
       <c r="J122" t="n">
-        <v>0.2180864984603487</v>
+        <v>0.2180438559685123</v>
       </c>
     </row>
     <row r="123">
@@ -5113,7 +5113,7 @@
         <v>0.188</v>
       </c>
       <c r="J123" t="n">
-        <v>0.04316700988178825</v>
+        <v>0.04315520271554419</v>
       </c>
     </row>
     <row r="124">
@@ -5151,7 +5151,7 @@
         <v>0.073</v>
       </c>
       <c r="J124" t="n">
-        <v>0.008354539871618308</v>
+        <v>0.0082583363228712</v>
       </c>
     </row>
     <row r="125">
@@ -5227,7 +5227,7 @@
         <v>0.188</v>
       </c>
       <c r="J126" t="n">
-        <v>0.4053626939321028</v>
+        <v>0.4053410467517753</v>
       </c>
     </row>
     <row r="127">
@@ -5303,7 +5303,7 @@
         <v>0.073</v>
       </c>
       <c r="J128" t="n">
-        <v>-0.003165669172762418</v>
+        <v>-0.003204083349782384</v>
       </c>
     </row>
     <row r="129">
@@ -5341,7 +5341,7 @@
         <v>0.309</v>
       </c>
       <c r="J129" t="n">
-        <v>0.03465876500810812</v>
+        <v>0.03466907120609651</v>
       </c>
     </row>
     <row r="130">
@@ -5376,10 +5376,10 @@
         </is>
       </c>
       <c r="I130" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J130" t="n">
-        <v>0.4639289827682891</v>
+        <v>0.46397043003758</v>
       </c>
     </row>
     <row r="131">
@@ -5414,10 +5414,10 @@
         </is>
       </c>
       <c r="I131" t="n">
-        <v>0.298</v>
+        <v>0.297</v>
       </c>
       <c r="J131" t="n">
-        <v>0.474913818154078</v>
+        <v>0.4749081316104607</v>
       </c>
     </row>
     <row r="132">
@@ -5455,7 +5455,7 @@
         <v>0.277</v>
       </c>
       <c r="J132" t="n">
-        <v>0.3238845461197721</v>
+        <v>0.3238956940761398</v>
       </c>
     </row>
     <row r="133">
@@ -5493,7 +5493,7 @@
         <v>0.623</v>
       </c>
       <c r="J133" t="n">
-        <v>0.7537992518593929</v>
+        <v>0.7537922359360606</v>
       </c>
     </row>
     <row r="134">
@@ -5531,7 +5531,7 @@
         <v>0.188</v>
       </c>
       <c r="J134" t="n">
-        <v>0.2649540865670368</v>
+        <v>0.2648577132674607</v>
       </c>
     </row>
     <row r="135">
@@ -5569,7 +5569,7 @@
         <v>0.478</v>
       </c>
       <c r="J135" t="n">
-        <v>0.4332059722857927</v>
+        <v>0.4332134325842215</v>
       </c>
     </row>
     <row r="136">
@@ -5607,7 +5607,7 @@
         <v>0.134</v>
       </c>
       <c r="J136" t="n">
-        <v>-0.1127665883725204</v>
+        <v>-0.1127492619789603</v>
       </c>
     </row>
     <row r="137">
@@ -5642,10 +5642,10 @@
         </is>
       </c>
       <c r="I137" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J137" t="n">
-        <v>0.431461878288157</v>
+        <v>0.4314643318462793</v>
       </c>
     </row>
     <row r="138">
@@ -5683,7 +5683,7 @@
         <v>0.252</v>
       </c>
       <c r="J138" t="n">
-        <v>0.05830847765085004</v>
+        <v>0.05830586168058267</v>
       </c>
     </row>
     <row r="139">
@@ -5721,7 +5721,7 @@
         <v>0.134</v>
       </c>
       <c r="J139" t="n">
-        <v>0.2747661474562089</v>
+        <v>0.2747243817280189</v>
       </c>
     </row>
     <row r="140">
@@ -5759,7 +5759,7 @@
         <v>0.148</v>
       </c>
       <c r="J140" t="n">
-        <v>0.1621491943872339</v>
+        <v>0.1621929635881888</v>
       </c>
     </row>
     <row r="141">
@@ -5797,7 +5797,7 @@
         <v>0.203</v>
       </c>
       <c r="J141" t="n">
-        <v>0.05758701261209637</v>
+        <v>0.05755448922871158</v>
       </c>
     </row>
     <row r="142">
@@ -5835,7 +5835,7 @@
         <v>0.505</v>
       </c>
       <c r="J142" t="n">
-        <v>0.5772344955966715</v>
+        <v>0.5772295316352288</v>
       </c>
     </row>
     <row r="143">
@@ -5870,10 +5870,10 @@
         </is>
       </c>
       <c r="I143" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J143" t="n">
-        <v>0.227281379036027</v>
+        <v>0.2256141425221004</v>
       </c>
     </row>
     <row r="144">
@@ -5908,10 +5908,10 @@
         </is>
       </c>
       <c r="I144" t="n">
-        <v>0.298</v>
+        <v>0.297</v>
       </c>
       <c r="J144" t="n">
-        <v>0.3451864869588811</v>
+        <v>0.3451780314109147</v>
       </c>
     </row>
     <row r="145">
@@ -5946,10 +5946,10 @@
         </is>
       </c>
       <c r="I145" t="n">
-        <v>0.298</v>
+        <v>0.297</v>
       </c>
       <c r="J145" t="n">
-        <v>0.2760017483674853</v>
+        <v>0.2760130722342768</v>
       </c>
     </row>
     <row r="146">
@@ -5987,7 +5987,7 @@
         <v>0.203</v>
       </c>
       <c r="J146" t="n">
-        <v>0.2361164744625469</v>
+        <v>0.2360268391411614</v>
       </c>
     </row>
     <row r="147">
@@ -6025,7 +6025,7 @@
         <v>0.134</v>
       </c>
       <c r="J147" t="n">
-        <v>0.1764197324924833</v>
+        <v>0.1764195050571176</v>
       </c>
     </row>
     <row r="148">
@@ -6063,7 +6063,7 @@
         <v>0.148</v>
       </c>
       <c r="J148" t="n">
-        <v>-0.05771998240783974</v>
+        <v>-0.05771101396237924</v>
       </c>
     </row>
     <row r="149">
@@ -6101,7 +6101,7 @@
         <v>0.134</v>
       </c>
       <c r="J149" t="n">
-        <v>0.1786216493665166</v>
+        <v>0.178609980221771</v>
       </c>
     </row>
     <row r="150">
@@ -6177,7 +6177,7 @@
         <v>0.177</v>
       </c>
       <c r="J151" t="n">
-        <v>0.2330864669125591</v>
+        <v>0.2330839786091164</v>
       </c>
     </row>
     <row r="152">
@@ -6212,10 +6212,10 @@
         </is>
       </c>
       <c r="I152" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="J152" t="n">
-        <v>0.2943217302769264</v>
+        <v>0.2943156614024233</v>
       </c>
     </row>
     <row r="153">
@@ -6250,10 +6250,10 @@
         </is>
       </c>
       <c r="I153" t="n">
-        <v>0.298</v>
+        <v>0.297</v>
       </c>
       <c r="J153" t="n">
-        <v>0.2678859032461168</v>
+        <v>0.2679526827183633</v>
       </c>
     </row>
     <row r="154">
@@ -6291,7 +6291,7 @@
         <v>0.303</v>
       </c>
       <c r="J154" t="n">
-        <v>0.03885580988823681</v>
+        <v>0.03886474090408995</v>
       </c>
     </row>
     <row r="155">
@@ -6329,7 +6329,7 @@
         <v>0.188</v>
       </c>
       <c r="J155" t="n">
-        <v>0.02576856424967135</v>
+        <v>0.02573408816647139</v>
       </c>
     </row>
     <row r="156">
@@ -6367,7 +6367,7 @@
         <v>0.148</v>
       </c>
       <c r="J156" t="n">
-        <v>-0.02592980520787887</v>
+        <v>-0.02591264463275347</v>
       </c>
     </row>
     <row r="157">
@@ -6402,10 +6402,10 @@
         </is>
       </c>
       <c r="I157" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J157" t="n">
-        <v>0.2170175721237151</v>
+        <v>0.2188484571134909</v>
       </c>
     </row>
     <row r="158">
@@ -6443,7 +6443,7 @@
         <v>0.148</v>
       </c>
       <c r="J158" t="n">
-        <v>0.2487814493386147</v>
+        <v>0.2487270032837418</v>
       </c>
     </row>
     <row r="159">
@@ -6481,7 +6481,7 @@
         <v>0.177</v>
       </c>
       <c r="J159" t="n">
-        <v>0.09370996959553195</v>
+        <v>0.09365804532186177</v>
       </c>
     </row>
     <row r="160">
@@ -6519,7 +6519,7 @@
         <v>0.303</v>
       </c>
       <c r="J160" t="n">
-        <v>0.3794695051740847</v>
+        <v>0.3794525137407735</v>
       </c>
     </row>
     <row r="161">
@@ -6554,10 +6554,10 @@
         </is>
       </c>
       <c r="I161" t="n">
-        <v>0.298</v>
+        <v>0.297</v>
       </c>
       <c r="J161" t="n">
-        <v>0.3866705208625674</v>
+        <v>0.3866628078194077</v>
       </c>
     </row>
     <row r="162">
@@ -6592,10 +6592,10 @@
         </is>
       </c>
       <c r="I162" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J162" t="n">
-        <v>0.4088194363562703</v>
+        <v>0.4088297105445195</v>
       </c>
     </row>
     <row r="163">
@@ -6630,10 +6630,10 @@
         </is>
       </c>
       <c r="I163" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J163" t="n">
-        <v>0.4412824560336345</v>
+        <v>0.4398763346224171</v>
       </c>
     </row>
     <row r="164">
@@ -6671,7 +6671,7 @@
         <v>0.188</v>
       </c>
       <c r="J164" t="n">
-        <v>0.1827661125741168</v>
+        <v>0.182670149036062</v>
       </c>
     </row>
     <row r="165">
@@ -6709,7 +6709,7 @@
         <v>0.134</v>
       </c>
       <c r="J165" t="n">
-        <v>0.4085986444558704</v>
+        <v>0.4086199671472354</v>
       </c>
     </row>
     <row r="166">
@@ -6747,7 +6747,7 @@
         <v>0.432</v>
       </c>
       <c r="J166" t="n">
-        <v>0.5590321480189022</v>
+        <v>0.5590429321613626</v>
       </c>
     </row>
     <row r="167">
@@ -6785,7 +6785,7 @@
         <v>0.16</v>
       </c>
       <c r="J167" t="n">
-        <v>-0.04823233001509197</v>
+        <v>-0.04820288235235334</v>
       </c>
     </row>
     <row r="168">
@@ -6820,10 +6820,10 @@
         </is>
       </c>
       <c r="I168" t="n">
-        <v>0.396</v>
+        <v>0.395</v>
       </c>
       <c r="J168" t="n">
-        <v>0.2559954936563182</v>
+        <v>0.2559931288713875</v>
       </c>
     </row>
     <row r="169">
@@ -6861,7 +6861,7 @@
         <v>0.252</v>
       </c>
       <c r="J169" t="n">
-        <v>0.4369001724747012</v>
+        <v>0.4368438998785887</v>
       </c>
     </row>
     <row r="170">
@@ -6899,7 +6899,7 @@
         <v>0.275</v>
       </c>
       <c r="J170" t="n">
-        <v>0.3993873741738188</v>
+        <v>0.3990569004013871</v>
       </c>
     </row>
     <row r="171">
@@ -6937,7 +6937,7 @@
         <v>0.546</v>
       </c>
       <c r="J171" t="n">
-        <v>0.5344291275723119</v>
+        <v>0.5344562933862126</v>
       </c>
     </row>
     <row r="172">
@@ -6975,7 +6975,7 @@
         <v>0.277</v>
       </c>
       <c r="J172" t="n">
-        <v>0.2440058225427611</v>
+        <v>0.2440436675216786</v>
       </c>
     </row>
     <row r="173">
@@ -7010,10 +7010,10 @@
         </is>
       </c>
       <c r="I173" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J173" t="n">
-        <v>0.1098172304060437</v>
+        <v>0.112102830497141</v>
       </c>
     </row>
     <row r="174">
@@ -7048,10 +7048,10 @@
         </is>
       </c>
       <c r="I174" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J174" t="n">
-        <v>0.1439235960735294</v>
+        <v>0.1451268218510944</v>
       </c>
     </row>
     <row r="175">
@@ -7089,7 +7089,7 @@
         <v>0.432</v>
       </c>
       <c r="J175" t="n">
-        <v>0.5567854296274747</v>
+        <v>0.5567892488713136</v>
       </c>
     </row>
     <row r="176">
@@ -7127,7 +7127,7 @@
         <v>0.623</v>
       </c>
       <c r="J176" t="n">
-        <v>0.7397852002974307</v>
+        <v>0.7397761206878575</v>
       </c>
     </row>
     <row r="177">
@@ -7165,7 +7165,7 @@
         <v>0.151</v>
       </c>
       <c r="J177" t="n">
-        <v>0.2273250854060668</v>
+        <v>0.2273278746873446</v>
       </c>
     </row>
     <row r="178">
@@ -7203,7 +7203,7 @@
         <v>0.303</v>
       </c>
       <c r="J178" t="n">
-        <v>0.2466094490418907</v>
+        <v>0.2465861872507433</v>
       </c>
     </row>
     <row r="179">
@@ -7241,7 +7241,7 @@
         <v>0.16</v>
       </c>
       <c r="J179" t="n">
-        <v>0.2992365922004274</v>
+        <v>0.2992708635541579</v>
       </c>
     </row>
     <row r="180">
@@ -7279,7 +7279,7 @@
         <v>0.277</v>
       </c>
       <c r="J180" t="n">
-        <v>0.3623753228433881</v>
+        <v>0.3623997313705833</v>
       </c>
     </row>
     <row r="181">
@@ -7317,7 +7317,7 @@
         <v>0.148</v>
       </c>
       <c r="J181" t="n">
-        <v>0.4087842651044669</v>
+        <v>0.4087674140078181</v>
       </c>
     </row>
     <row r="182">
@@ -7355,7 +7355,7 @@
         <v>0.303</v>
       </c>
       <c r="J182" t="n">
-        <v>0.370338072519153</v>
+        <v>0.3703491704616199</v>
       </c>
     </row>
     <row r="183">
@@ -7393,7 +7393,7 @@
         <v>0.16</v>
       </c>
       <c r="J183" t="n">
-        <v>0.2647742040636606</v>
+        <v>0.2647810281568248</v>
       </c>
     </row>
     <row r="184">
@@ -7431,7 +7431,7 @@
         <v>0.148</v>
       </c>
       <c r="J184" t="n">
-        <v>0.004970741975489096</v>
+        <v>0.004859722060753417</v>
       </c>
     </row>
     <row r="185">
@@ -7469,7 +7469,7 @@
         <v>0.134</v>
       </c>
       <c r="J185" t="n">
-        <v>-0.04792183556344386</v>
+        <v>-0.04792450998496866</v>
       </c>
     </row>
     <row r="186">
@@ -7504,10 +7504,10 @@
         </is>
       </c>
       <c r="I186" t="n">
-        <v>0.168</v>
+        <v>0.17</v>
       </c>
       <c r="J186" t="n">
-        <v>0.1869631178472956</v>
+        <v>0.1859809522966333</v>
       </c>
     </row>
     <row r="187">
@@ -7545,7 +7545,7 @@
         <v>0.478</v>
       </c>
       <c r="J187" t="n">
-        <v>0.5218485903999984</v>
+        <v>0.5218935442850676</v>
       </c>
     </row>
     <row r="188">
@@ -7583,7 +7583,7 @@
         <v>0.505</v>
       </c>
       <c r="J188" t="n">
-        <v>0.607496609620796</v>
+        <v>0.6074933946085957</v>
       </c>
     </row>
     <row r="189">
@@ -7621,7 +7621,7 @@
         <v>0.505</v>
       </c>
       <c r="J189" t="n">
-        <v>0.6146049444680578</v>
+        <v>0.6146017680457476</v>
       </c>
     </row>
     <row r="190">
@@ -7659,7 +7659,7 @@
         <v>-0.024</v>
       </c>
       <c r="J190" t="n">
-        <v>-0.1110867383015212</v>
+        <v>-0.1110989130225092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>